<commit_message>
Created powerpoint and updated todo list
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Winter.xlsx
+++ b/Documentation/TODO List Winter.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="0" yWindow="132" windowWidth="22980" windowHeight="9468"/>
   </bookViews>
   <sheets>
-    <sheet name="12-12-14 to 12-19-14" sheetId="13" r:id="rId1"/>
+    <sheet name="12-18-14 to 1-8-15" sheetId="14" r:id="rId1"/>
+    <sheet name="12-12-14 to 12-19-14" sheetId="13" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -117,7 +118,73 @@
     <t>Look into JCI batteries</t>
   </si>
   <si>
-    <t>Batteries get!</t>
+    <t>It's the adiabatic index</t>
+  </si>
+  <si>
+    <t>Batteries talk!</t>
+  </si>
+  <si>
+    <t>Ask Milwaukee tool about batteries?</t>
+  </si>
+  <si>
+    <t>Somebody?</t>
+  </si>
+  <si>
+    <t>Ask Dr. Rodriguez what he think</t>
+  </si>
+  <si>
+    <t>Develop robot control mechanism</t>
+  </si>
+  <si>
+    <t>Finish deriving equations and simulation</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Ron, Logan, Justin</t>
+  </si>
+  <si>
+    <t>A microcontroller running matlab can be controlled by a laptop wirelessly</t>
+  </si>
+  <si>
+    <t>Finish developing state-based model and integrate it with the simulation</t>
+  </si>
+  <si>
+    <t>Put masses and moments of inertia in excel spreadhseet</t>
+  </si>
+  <si>
+    <t>Input required masses and intertias into an excel file</t>
+  </si>
+  <si>
+    <t>Materials science research</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>List of lightweight and cheap sheet materials that can be used for component mounting inside chassis</t>
+  </si>
+  <si>
+    <t>Whatever Dr Rodriguez says</t>
+  </si>
+  <si>
+    <t>The truth</t>
+  </si>
+  <si>
+    <t>Styrofoam model?</t>
+  </si>
+  <si>
+    <t>Please?</t>
+  </si>
+  <si>
+    <t>Start presentation powerpoint</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Individual sections finished per person, 3 minutes max per section</t>
   </si>
 </sst>
 </file>
@@ -149,12 +216,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,6 +259,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,79 +603,68 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -598,35 +674,187 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="64" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="9" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -635,14 +863,14 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>32</v>
+      <c r="C19" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memo and TODO list update 1/8/2015
Memo updated

TODO list updated
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Winter.xlsx
+++ b/Documentation/TODO List Winter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Documents\Classes\AgileRoboticControls\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\Git\AgileRoboticControls\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -203,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +227,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +253,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,6 +303,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +614,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +645,7 @@
       <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -647,7 +675,7 @@
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -658,7 +686,7 @@
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -680,7 +708,7 @@
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="13" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="2" t="s">

</xml_diff>

<commit_message>
Powerpoint, TODO List, Memo4
Powerpoint controls and software slides added

TODO list (color updated)

Memo 4 Goals removed since they have not been decided.
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Winter.xlsx
+++ b/Documentation/TODO List Winter.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\Git\AgileRoboticControls\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="192" windowWidth="22980" windowHeight="9408"/>
   </bookViews>
@@ -229,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,12 +256,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,9 +298,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,7 +396,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,7 +608,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +650,7 @@
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>56</v>
       </c>
     </row>
@@ -659,7 +658,7 @@
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -670,7 +669,7 @@
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -681,7 +680,7 @@
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -692,7 +691,7 @@
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -703,7 +702,7 @@
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="2" t="s">

</xml_diff>

<commit_message>
TODO list updated for Advisor meeting
TODO list updated 2015/1/13

Memo 4 updated
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Winter.xlsx
+++ b/Documentation/TODO List Winter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Documents\Classes\AgileRoboticControls\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\Git\AgileRoboticControls\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -198,6 +198,69 @@
   </si>
   <si>
     <t>Logan, Tyler</t>
+  </si>
+  <si>
+    <t>Research Tasks</t>
+  </si>
+  <si>
+    <t>Compressors</t>
+  </si>
+  <si>
+    <t>Common compressors with pressures, cost, ect…</t>
+  </si>
+  <si>
+    <t>Cylinders</t>
+  </si>
+  <si>
+    <t>Cost, Stroke Length, Bore size</t>
+  </si>
+  <si>
+    <t>Pick foot rubber</t>
+  </si>
+  <si>
+    <t>Dynamic Model</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Updates completed</t>
+  </si>
+  <si>
+    <t>Foot selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication System </t>
+  </si>
+  <si>
+    <t>Constructed Communication System</t>
+  </si>
+  <si>
+    <t>Debug Panel</t>
+  </si>
+  <si>
+    <t>Start design of debug panel</t>
+  </si>
+  <si>
+    <t>Verify dynamic equations</t>
+  </si>
+  <si>
+    <t>Problems found or no?</t>
+  </si>
+  <si>
+    <t>Scan the feedback from presentation</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Project Presentation feedback on Git</t>
+  </si>
+  <si>
+    <t>Design foot</t>
+  </si>
+  <si>
+    <t>Foot Designed</t>
   </si>
 </sst>
 </file>
@@ -606,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,108 +701,106 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>58</v>
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>56</v>
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>57</v>
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>3</v>
+        <v>64</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>49</v>
+      <c r="A13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>